<commit_message>
Moved some media around. Added in upvote/downvote functionality in the javascript. Added curation functionality in the javascript - to be implemented.
</commit_message>
<xml_diff>
--- a/Content_info.xlsx
+++ b/Content_info.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aidan\Google Drive\University\2016 Sem2\DECO3500\DECO3500 Group Folder\First Prototype\Backend design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TEMPORARY GIT\DECO3500\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Upvotes</t>
   </si>
@@ -93,24 +93,6 @@
     <t>Business</t>
   </si>
   <si>
-    <t>0001</t>
-  </si>
-  <si>
-    <t>0002</t>
-  </si>
-  <si>
-    <t>0003</t>
-  </si>
-  <si>
-    <t>0004</t>
-  </si>
-  <si>
-    <t>0005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Money bag: Police raid on anti-corruption official uncovers over $120mn in cash </t>
-  </si>
-  <si>
     <t>https://www.rt.com/news/358891-russia-corruption-officer-dollars/</t>
   </si>
   <si>
@@ -151,24 +133,100 @@
   </si>
   <si>
     <t>Food, Business</t>
+  </si>
+  <si>
+    <t>Money bag: Police raid on anti-corruption official uncovers over $120mn in cash</t>
+  </si>
+  <si>
+    <t>Here's all the drama that you missed from the "The Bachelor" Australia Finale</t>
+  </si>
+  <si>
+    <t>https://www.buzzfeed.com/tahliapritchard/i-am-so-shook?utm_term=.ueJPK2aMW#.isLRJbVBp</t>
+  </si>
+  <si>
+    <t>shelby_pye</t>
+  </si>
+  <si>
+    <t>Nadal stops match so distraught mother can find lost child</t>
+  </si>
+  <si>
+    <t>https://au.sports.yahoo.com/tennis/a/32758243/rafael-nadal-stops-match-so-mother-can-find-lost-child/#page1</t>
+  </si>
+  <si>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>Adventure Time is Coming to and End in 2018</t>
+  </si>
+  <si>
+    <t>http://comicbook.com/2016/09/29/adventure-time-is-coming-to-an-end-in-2018/</t>
+  </si>
+  <si>
+    <t>This is exactly what you should be eating in exam time</t>
+  </si>
+  <si>
+    <t>https://www.buzzfeed.com/gyanyankovich/eat-your-way-through-exams?utm_term=.mbqoKpW7M#.kugPyLNgX</t>
+  </si>
+  <si>
+    <t>Food, Science</t>
+  </si>
+  <si>
+    <t>South Australia belted by second storm in 24 hours with winds of up to 140km/h</t>
+  </si>
+  <si>
+    <t>https://www.theguardian.com/australia-news/2016/sep/29/south-australia-on-alert-again-as-adelaide-braces-for-strongest-storm-on-record</t>
+  </si>
+  <si>
+    <t>Science, Local</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Note 7 banned on all U.S. flights due to fire hazard</t>
+  </si>
+  <si>
+    <t>http://www.usatoday.com/story/news/2016/10/14/dot-bans-samsung-galaxy-note-7-flights/92066322/</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Cahill scores 40m screamer in City debut</t>
+  </si>
+  <si>
+    <t>https://au.sports.yahoo.com/football/a/32911441/tim-cahill-scores-40-goal-for-melbourne-city-debut-melbourne-derby/#page1</t>
+  </si>
+  <si>
+    <t>Olivia Wilde and Jason Sudeikis welcome second child</t>
+  </si>
+  <si>
+    <t>http://www.hollywoodreporter.com/news/olivia-wilde-jason-sudeikis-second-938619</t>
+  </si>
+  <si>
+    <t>This Is Why Mike Baird Overturned The Greyhound Ban</t>
+  </si>
+  <si>
+    <t>https://www.buzzfeed.com/ginarushton/this-is-why-mike-baird-overturned-the-greyhound-ban?utm_term=.nrbm6ZM1y#.rn5lgDQJR</t>
+  </si>
+  <si>
+    <t>Politics</t>
+  </si>
+  <si>
+    <t>Hillary Clinton Finally Addressed That Creepy Hovering Trump Did In The Debate</t>
+  </si>
+  <si>
+    <t>https://www.buzzfeed.com/erinlarosa/hillary-clinton-finally-addressed-that-creepy-hovering-trump?utm_term=.rjy4JlB3z#.dhD9Gqdlk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
     </font>
     <font>
       <sz val="9"/>
@@ -183,27 +241,71 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12.1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arimo"/>
+    </font>
+    <font>
+      <sz val="12.1"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCFBFB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -229,24 +331,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,237 +697,554 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A2" sqref="A2:J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.25" customWidth="1"/>
+    <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4">
+        <v>42653</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="5">
+        <v>42683.888194444444</v>
+      </c>
+      <c r="H2" s="6">
+        <v>18</v>
+      </c>
+      <c r="I2" s="6">
+        <v>2</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0.69896179359999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4">
+        <v>42683</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5">
+        <v>42683.895833333336</v>
+      </c>
+      <c r="H3" s="6">
+        <v>5</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.56550850519999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4">
+        <v>42652</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="5">
+        <v>42683.90347222222</v>
+      </c>
+      <c r="H4" s="6">
+        <v>3</v>
+      </c>
+      <c r="I4" s="6">
+        <v>6</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.1205815987</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4">
+        <v>42683</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="8">
-        <v>42653</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="6">
-        <v>42624.888194444444</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="J2" s="1">
-        <f t="shared" ref="J2:J11" si="0">IFERROR(((H2 + 1.9208) / (H2 + I2) - 1.96 * SQRT((H2 *  I2) / (H2 +  I2) + 0.9604) / (H2 +  I2)) / (1 + 3.8416 / (H2 +  I2)),0)</f>
+      <c r="G5" s="5">
+        <v>42683.911111111112</v>
+      </c>
+      <c r="H5" s="6">
+        <v>4</v>
+      </c>
+      <c r="I5" s="6">
+        <v>2</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.29998832130000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4">
+        <v>42591</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="5">
+        <v>42683.918749999997</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
+        <v>15</v>
+      </c>
+      <c r="J6" s="7">
+        <v>1.111905731E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="8">
+        <v>42628</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="5">
+        <v>42683.926388888889</v>
+      </c>
+      <c r="H7" s="6">
+        <v>10</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0.62263537449999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="8">
+        <v>42642</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="5">
+        <v>42683.934027777781</v>
+      </c>
+      <c r="H8" s="6">
+        <v>3</v>
+      </c>
+      <c r="I8" s="6">
+        <v>2</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0.23071993220000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="8">
+        <v>42642</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="5">
+        <v>42683.941666666666</v>
+      </c>
+      <c r="H9" s="6">
+        <v>5</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.43649056339999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="8">
+        <v>42641</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="5">
+        <v>42683.949305555558</v>
+      </c>
+      <c r="H10" s="6">
+        <v>8</v>
+      </c>
+      <c r="I10" s="6">
+        <v>3</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0.43434970699999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16.5" thickBot="1">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="8">
+        <v>42642</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="5">
+        <v>42683.956944444442</v>
+      </c>
+      <c r="H11" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="7" t="s">
+      <c r="I11" s="6">
+        <v>20</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="111" thickBot="1">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="8">
+        <v>42657</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="5">
+        <v>42683.964583333334</v>
+      </c>
+      <c r="H12" s="11">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="8">
-        <v>42624</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="6">
-        <v>42624.895833333336</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="J3" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="7" t="s">
+      <c r="I12" s="6">
+        <v>2</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0.60058092240000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="63.75" thickBot="1">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="8">
+        <v>42658</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="5">
+        <v>42683.972222222219</v>
+      </c>
+      <c r="H13" s="11">
+        <v>2</v>
+      </c>
+      <c r="I13" s="6">
+        <v>3</v>
+      </c>
+      <c r="J13" s="7">
+        <v>0.11761823120000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="65.25" thickBot="1">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="8">
-        <v>42623</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="6">
-        <v>42624.903472280093</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="J4" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="7" t="s">
+      <c r="B14" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="8">
+        <v>42658</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="5">
+        <v>42683.979861111111</v>
+      </c>
+      <c r="H14" s="11">
+        <v>30</v>
+      </c>
+      <c r="I14" s="6">
+        <v>54</v>
+      </c>
+      <c r="J14" s="7">
+        <v>0.26299209330000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="95.25" thickBot="1">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="8">
-        <v>42624</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="6">
-        <v>42624.911111226851</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="J5" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="7" t="s">
+      <c r="B15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="8">
+        <v>42657</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="5">
+        <v>42683.987500000003</v>
+      </c>
+      <c r="H15" s="11">
+        <v>14</v>
+      </c>
+      <c r="I15" s="6">
+        <v>8</v>
+      </c>
+      <c r="J15" s="7">
+        <v>0.4295134934</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="142.5" thickBot="1">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="8">
+        <v>42659</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="8">
-        <v>42621</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="6">
-        <v>42624.918750173609</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="J6" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="7"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="2"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="7"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="2"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="7"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="2"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="7"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="2"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="7"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="2"/>
-      <c r="J11" s="1"/>
+      <c r="F16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="5">
+        <v>42683.995138888888</v>
+      </c>
+      <c r="H16" s="11">
+        <v>9</v>
+      </c>
+      <c r="I16" s="6">
+        <v>1</v>
+      </c>
+      <c r="J16" s="7">
+        <v>0.59584361450000001</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:K11">
     <sortCondition descending="1" ref="J2:J11"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1" location=".isLRJbVBp" display="https://www.buzzfeed.com/tahliapritchard/i-am-so-shook?utm_term=.ueJPK2aMW - .isLRJbVBp"/>
+    <hyperlink ref="D8" r:id="rId2" location="page1" display="https://au.sports.yahoo.com/tennis/a/32758243/rafael-nadal-stops-match-so-mother-can-find-lost-child/ - page1"/>
+    <hyperlink ref="D9" r:id="rId3"/>
+    <hyperlink ref="D10" r:id="rId4" location=".kugPyLNgX" display="https://www.buzzfeed.com/gyanyankovich/eat-your-way-through-exams?utm_term=.mbqoKpW7M - .kugPyLNgX"/>
+    <hyperlink ref="D11" r:id="rId5"/>
+    <hyperlink ref="D12" r:id="rId6"/>
+    <hyperlink ref="D13" r:id="rId7" location="page1" display="https://au.sports.yahoo.com/football/a/32911441/tim-cahill-scores-40-goal-for-melbourne-city-debut-melbourne-derby/ - page1"/>
+    <hyperlink ref="D14" r:id="rId8"/>
+    <hyperlink ref="D15" r:id="rId9" location=".rn5lgDQJR" display="https://www.buzzfeed.com/ginarushton/this-is-why-mike-baird-overturned-the-greyhound-ban?utm_term=.nrbm6ZM1y - .rn5lgDQJR"/>
+    <hyperlink ref="D16" r:id="rId10" location=".dhD9Gqdlk" display="https://www.buzzfeed.com/erinlarosa/hillary-clinton-finally-addressed-that-creepy-hovering-trump?utm_term=.rjy4JlB3z - .dhD9Gqdlk"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>